<commit_message>
Apply OutputFormatter for templateExport
</commit_message>
<xml_diff>
--- a/samples/DotNetCoreSample/Templates/testTemplate.xlsx
+++ b/samples/DotNetCoreSample/Templates/testTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\sources\WeihanLi.Npoi\samples\DotNetCoreSample\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BD2BEF2-7FB8-4EC5-95C4-00CC6A710BC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A01118D9-49AE-4A32-861C-0AE994D209D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1545" yWindow="3053" windowWidth="15390" windowHeight="9532" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SystemSettings" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>$(Global:Title)</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -64,6 +64,10 @@
   </si>
   <si>
     <t>&lt;Data&gt;$(Data:SettingId)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>$(Data:Enabled)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -412,7 +416,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -436,7 +440,9 @@
         <v>9</v>
       </c>
       <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
+      <c r="C2" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>

</xml_diff>